<commit_message>
fix(GUI/API): Report integration and total value of transactions
</commit_message>
<xml_diff>
--- a/API/dat_pl.xlsx
+++ b/API/dat_pl.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TI\Desktop\Proyectos\Fullstack\Angular -- Django\EcommercePlatform\API\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alan8\OneDrive\Escritorio\Nueva carpeta\EcommercePlatform\API\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19455" windowHeight="10050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19452" windowHeight="10056"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Id</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>Fecha</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -73,7 +76,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -81,16 +84,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,39 +394,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -412,6 +435,17 @@
       <c r="F2" s="2"/>
       <c r="G2" s="1"/>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H3" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H4" s="5">
+        <f>SUM(F2:F1000)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>